<commit_message>
Wrapped up lab scripts, just need to write out transfer functions
</commit_message>
<xml_diff>
--- a/421Lab/Lab 3/data/rawdata.xlsx
+++ b/421Lab/Lab 3/data/rawdata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class Work\Current\ME421\421Lab\Lab 3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{033D10BB-4089-4BD7-87C3-645E1937E7FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54694C5-F33E-45FE-B221-DCDF316F31C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="1056" windowWidth="23040" windowHeight="12204"/>
+    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEK0000" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -169,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1004,12 +1015,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26372,5 +26388,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>